<commit_message>
backing up progress (again)
</commit_message>
<xml_diff>
--- a/data/metaanalysis-datasets.xlsx
+++ b/data/metaanalysis-datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmanning/prediction-retrodiction-paper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF94A559-A04F-5D4F-ADB6-5611F1FF352B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4245AF-2789-C04F-AAD3-C9AF7CF4CB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42160" yWindow="4160" windowWidth="31540" windowHeight="25680" xr2:uid="{9945677C-6850-0245-8B03-A32B92AF8A89}"/>
   </bookViews>
@@ -268,9 +268,6 @@
     </r>
   </si>
   <si>
-    <t>A collection of scripts from roughly 1000 popular movies.</t>
-  </si>
-  <si>
     <t>https://imsdb.com</t>
   </si>
   <si>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>Transcript</t>
+  </si>
+  <si>
+    <t>A collection of transcripts from roughly 1000 popular movies.</t>
   </si>
 </sst>
 </file>
@@ -743,7 +743,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -754,6 +754,7 @@
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="5" width="45.1640625" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -773,16 +774,16 @@
         <v>60</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>73</v>
-      </c>
       <c r="I1" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="85" x14ac:dyDescent="0.2">
@@ -796,21 +797,23 @@
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="7">
         <v>1091</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="I2" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="I2" s="7">
+        <v>26023348</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -829,15 +832,17 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="7">
         <v>304713</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="I3" s="7">
+        <v>3209921</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -856,15 +861,17 @@
         <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="7">
         <v>122646</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="I4" s="7">
+        <v>2052779</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -883,15 +890,17 @@
         <v>28</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G5" s="7">
         <v>1700789</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="I5" s="7">
+        <v>71889094</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -910,15 +919,17 @@
         <v>32</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G6" s="7">
         <v>163948</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="I6" s="7">
+        <v>7043118</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -937,15 +948,17 @@
         <v>61</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G7" s="7">
         <v>20932</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="I7" s="7">
+        <v>351759</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -964,15 +977,17 @@
         <v>38</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G8" s="7">
         <v>26562</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1898509</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="153" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -991,15 +1006,17 @@
         <v>43</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" s="7">
         <v>8009</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I9" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="I9" s="7">
+        <v>45989</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -1018,15 +1035,17 @@
         <v>55</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="7">
         <v>6</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="I10" s="7"/>
+        <v>73</v>
+      </c>
+      <c r="I10" s="7">
+        <v>19197</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -1045,15 +1064,17 @@
         <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11" s="7">
         <v>67373</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I11" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="I11" s="7">
+        <v>622894</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -1063,7 +1084,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>5</v>
@@ -1072,15 +1093,17 @@
         <v>6</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G12" s="7">
         <v>14773741</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="I12" s="7">
+        <v>327519461</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -1099,15 +1122,17 @@
         <v>19</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G13" s="7">
         <v>74468</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I13" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="I13" s="7">
+        <v>3080662</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F13">

</xml_diff>

<commit_message>
backing up meta analysis
</commit_message>
<xml_diff>
--- a/data/metaanalysis-datasets.xlsx
+++ b/data/metaanalysis-datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmanning/prediction-retrodiction-paper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4245AF-2789-C04F-AAD3-C9AF7CF4CB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3039757-0C46-3342-83AA-8A7F8B77FCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42160" yWindow="4160" windowWidth="31540" windowHeight="25680" xr2:uid="{9945677C-6850-0245-8B03-A32B92AF8A89}"/>
+    <workbookView xWindow="30240" yWindow="4520" windowWidth="31540" windowHeight="25680" xr2:uid="{9945677C-6850-0245-8B03-A32B92AF8A89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
   <si>
     <t>Internet Movie Script Database</t>
   </si>
@@ -306,6 +306,45 @@
   <si>
     <t>A collection of transcripts from roughly 1000 popular movies.</t>
   </si>
+  <si>
+    <t>Results URL</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/to0642t939pvrtz1tka9y/chair_results.pkl?rlkey=sqz65t6sap29fkedwd7vwk3w6&amp;dl=1</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/mkxc114g90rifsmzm881f/friends_results.pkl?rlkey=53qf44bwl2668h4irz14bf1ig&amp;dl=1</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/prk03sodn4pg8954cx9pa/gap_results.pkl?rlkey=wj2mngehnrm52thoetrkw22u1&amp;dl=1</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/s/jz15wcsceacaqva/gutenberg_results.pkl?dl=1</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/3gq5ieq7l25719if3my1f/imsdb_results.pkl?rlkey=01fjsk43sb8g05ccioysj0a7i&amp;dl=1</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/3d4eha6r6xop7h0u1shgg/iq2_results.pkl?rlkey=qhaltntbg03len7bqqrwcpgjw&amp;dl=1</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/arxkyhub2fi6qh5t79pfi/movies_results.pkl?rlkey=wmpf6aufzd2q86yju990a9keo&amp;dl=1</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/zmumd8uno58cqzoptr08m/pfg_results.pkl?rlkey=b4n8b7nh92rwgo7s91hgj7087&amp;dl=1</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/p999uknmzhx6f49ps5j0l/reddit_results.pkl?rlkey=lcmyva4t65dapqvw4y8fq8qrg&amp;dl=1</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/zxkvlrg4lfxcv7cjythp5/scotus_results.pkl?rlkey=krllpoa2jxvjlxrjxz6v9z2p5&amp;dl=1</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/d3g83mtz4mqhbpmxfco5t/tennis_results.pkl?rlkey=ti9lsz49zyv8ru77cn2240qk5&amp;dl=1</t>
+  </si>
+  <si>
+    <t>https://www.dropbox.com/scl/fi/1o7wqdlc1oo26y6ldpv8i/switchboard_results.pkl?rlkey=fetrrcp0vbsrmwydh39ikb918&amp;dl=1</t>
+  </si>
 </sst>
 </file>
 
@@ -313,7 +352,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -415,13 +454,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -740,24 +779,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D25515-4656-2741-9E2B-237B6AE02FCC}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="45.1640625" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="45.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -771,22 +808,25 @@
         <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -799,23 +839,26 @@
       <c r="D2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="7">
+      <c r="H2" s="7">
         <v>1091</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="7">
+      <c r="J2" s="7">
         <v>26023348</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -828,23 +871,26 @@
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="7">
+      <c r="H3" s="7">
         <v>304713</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="7">
+      <c r="J3" s="7">
         <v>3209921</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -857,23 +903,26 @@
       <c r="D4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="7">
+      <c r="H4" s="7">
         <v>122646</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I4" s="7">
+      <c r="J4" s="7">
         <v>2052779</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -886,23 +935,26 @@
       <c r="D5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G5" s="7">
+      <c r="H5" s="7">
         <v>1700789</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="7">
+      <c r="J5" s="7">
         <v>71889094</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -915,23 +967,26 @@
       <c r="D6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="7">
+      <c r="H6" s="7">
         <v>163948</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I6" s="7">
+      <c r="J6" s="7">
         <v>7043118</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -944,23 +999,26 @@
       <c r="D7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G7" s="7">
+      <c r="H7" s="7">
         <v>20932</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="7">
+      <c r="J7" s="7">
         <v>351759</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -973,23 +1031,26 @@
       <c r="D8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="7">
+      <c r="H8" s="7">
         <v>26562</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="7">
+      <c r="J8" s="7">
         <v>1898509</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="153" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -1002,23 +1063,26 @@
       <c r="D9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="7">
+      <c r="H9" s="7">
         <v>8009</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="7">
+      <c r="J9" s="7">
         <v>45989</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -1031,23 +1095,26 @@
       <c r="D10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G10" s="7">
+      <c r="H10" s="7">
         <v>6</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="7">
+      <c r="J10" s="7">
         <v>19197</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="119" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1060,23 +1127,26 @@
       <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="7">
+      <c r="H11" s="7">
         <v>67373</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="7">
+      <c r="J11" s="7">
         <v>622894</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -1089,23 +1159,26 @@
       <c r="D12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="7">
+      <c r="H12" s="7">
         <v>14773741</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="7">
+      <c r="J12" s="7">
         <v>327519461</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1118,25 +1191,28 @@
       <c r="D13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="7">
+      <c r="H13" s="7">
         <v>74468</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I13" s="7">
+      <c r="J13" s="7">
         <v>3080662</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F13">
-    <sortCondition ref="F2:F13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G13">
+    <sortCondition ref="G2:G13"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{DAB976B1-7D4D-CA45-897F-6B49F89B99B0}"/>
@@ -1163,6 +1239,18 @@
     <hyperlink ref="D8" r:id="rId22" xr:uid="{8298910B-EEF9-0542-AAFE-B82C82C70FFA}"/>
     <hyperlink ref="D9" r:id="rId23" xr:uid="{C59CBA13-85FC-3442-AD3A-A979419A95B9}"/>
     <hyperlink ref="C12" r:id="rId24" xr:uid="{4CC32479-6E9A-DB47-84A7-99A15CF50D53}"/>
+    <hyperlink ref="E10" r:id="rId25" xr:uid="{92E665AE-874A-D045-9E69-21FF4A55B164}"/>
+    <hyperlink ref="E11" r:id="rId26" xr:uid="{A60D7778-8A33-5D4A-A8A5-F3B234BC704E}"/>
+    <hyperlink ref="E9" r:id="rId27" xr:uid="{68F32D9C-25B0-8B4C-8A6E-132A2B1940C1}"/>
+    <hyperlink ref="E12" r:id="rId28" xr:uid="{C3EE849A-CF15-D344-952A-0D423B48033E}"/>
+    <hyperlink ref="E2" r:id="rId29" xr:uid="{FA01DA6C-769A-C845-8C29-BCFE2F4F353D}"/>
+    <hyperlink ref="E8" r:id="rId30" xr:uid="{A09D6B17-B8B0-A849-B188-4DA9F595CD9E}"/>
+    <hyperlink ref="E3" r:id="rId31" xr:uid="{A14F38A3-B342-2F4D-9ECB-B494C7B1B181}"/>
+    <hyperlink ref="E7" r:id="rId32" xr:uid="{E41C03C7-8790-E845-82B2-53B9AA354BA3}"/>
+    <hyperlink ref="E13" r:id="rId33" xr:uid="{E8D3AF70-D762-144C-A2FA-A3123DBB7C80}"/>
+    <hyperlink ref="E5" r:id="rId34" xr:uid="{6DF9768A-2F22-6B4C-B685-F29C1D70E2BF}"/>
+    <hyperlink ref="E6" r:id="rId35" xr:uid="{25906D58-518B-CB45-BA83-8F5AEB0F43F8}"/>
+    <hyperlink ref="E4" r:id="rId36" xr:uid="{03692A13-703B-234D-8A92-581EEEB7F4CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
updata meta-analysis code and data
</commit_message>
<xml_diff>
--- a/data/metaanalysis-datasets.xlsx
+++ b/data/metaanalysis-datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmanning/prediction-retrodiction-paper/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dartmouth-my.sharepoint.com/personal/f00481t_dartmouth_edu/Documents/CDL/prediction-retrodiction-paper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3039757-0C46-3342-83AA-8A7F8B77FCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{F3039757-0C46-3342-83AA-8A7F8B77FCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF9C8F39-EEA6-1B41-A0E3-6F64A9158A30}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="4520" windowWidth="31540" windowHeight="25680" xr2:uid="{9945677C-6850-0245-8B03-A32B92AF8A89}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="37300" windowHeight="21100" xr2:uid="{9945677C-6850-0245-8B03-A32B92AF8A89}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="92">
   <si>
     <t>Internet Movie Script Database</t>
   </si>
@@ -344,6 +344,18 @@
   </si>
   <si>
     <t>https://www.dropbox.com/scl/fi/1o7wqdlc1oo26y6ldpv8i/switchboard_results.pkl?rlkey=fetrrcp0vbsrmwydh39ikb918&amp;dl=1</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>scripted</t>
+  </si>
+  <si>
+    <t>spontaneous</t>
+  </si>
+  <si>
+    <t>constrained</t>
   </si>
 </sst>
 </file>
@@ -442,7 +454,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -462,6 +474,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -779,9 +794,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47D25515-4656-2741-9E2B-237B6AE02FCC}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -792,9 +809,10 @@
     <col min="6" max="6" width="45.1640625" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>56</v>
       </c>
@@ -825,8 +843,11 @@
       <c r="J1" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="K1" s="8" t="s">
+        <v>88</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -857,8 +878,11 @@
       <c r="J2" s="7">
         <v>26023348</v>
       </c>
+      <c r="K2" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -889,8 +913,11 @@
       <c r="J3" s="7">
         <v>3209921</v>
       </c>
+      <c r="K3" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -921,8 +948,11 @@
       <c r="J4" s="7">
         <v>2052779</v>
       </c>
+      <c r="K4" t="s">
+        <v>90</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -953,8 +983,11 @@
       <c r="J5" s="7">
         <v>71889094</v>
       </c>
+      <c r="K5" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -985,8 +1018,11 @@
       <c r="J6" s="7">
         <v>7043118</v>
       </c>
+      <c r="K6" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1017,8 +1053,11 @@
       <c r="J7" s="7">
         <v>351759</v>
       </c>
+      <c r="K7" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1049,8 +1088,11 @@
       <c r="J8" s="7">
         <v>1898509</v>
       </c>
+      <c r="K8" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" ht="153" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -1081,8 +1123,11 @@
       <c r="J9" s="7">
         <v>45989</v>
       </c>
+      <c r="K9" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>44</v>
       </c>
@@ -1113,8 +1158,11 @@
       <c r="J10" s="7">
         <v>19197</v>
       </c>
+      <c r="K10" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" ht="119" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1145,8 +1193,11 @@
       <c r="J11" s="7">
         <v>622894</v>
       </c>
+      <c r="K11" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -1177,8 +1228,11 @@
       <c r="J12" s="7">
         <v>327519461</v>
       </c>
+      <c r="K12" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="13" spans="1:10" ht="102" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1208,6 +1262,9 @@
       </c>
       <c r="J13" s="7">
         <v>3080662</v>
+      </c>
+      <c r="K13" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>